<commit_message>
settings for rdtookit capture form
</commit_message>
<xml_diff>
--- a/config/default/forms/app/rdtoolkit_capture.xlsx
+++ b/config/default/forms/app/rdtoolkit_capture.xlsx
@@ -12,14 +12,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mjI9PEisXNsbEpHvdg5lW5dRXFxGA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId8" roundtripDataSignature="AMtx7mi54nxa7l7nMIQbE1gs/WrDTtBIvQ=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="185">
   <si>
     <t>type</t>
   </si>
@@ -120,6 +120,9 @@
     <t>instance::tag</t>
   </si>
   <si>
+    <t>instance::type</t>
+  </si>
+  <si>
     <t>repeat_count</t>
   </si>
   <si>
@@ -225,13 +228,13 @@
     <t>Taken on</t>
   </si>
   <si>
-    <t>image</t>
-  </si>
-  <si>
     <t>rdtoolkit_image</t>
   </si>
   <si>
     <t>Image</t>
+  </si>
+  <si>
+    <t>binary</t>
   </si>
   <si>
     <t>end group</t>
@@ -1073,7 +1076,7 @@
     <col customWidth="1" min="22" max="22" width="73.86"/>
     <col customWidth="1" min="24" max="24" width="30.0"/>
     <col hidden="1" min="25" max="30" width="14.43"/>
-    <col customWidth="1" min="32" max="37" width="29.86"/>
+    <col customWidth="1" min="32" max="38" width="29.86"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -1176,14 +1179,17 @@
       <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="3"/>
+      <c r="AJ1" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="AK1" s="3"/>
+      <c r="AL1" s="3"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="4"/>
@@ -1191,13 +1197,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
@@ -1217,7 +1223,7 @@
       <c r="S3" s="7"/>
       <c r="T3" s="7"/>
       <c r="U3" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="V3" s="9"/>
       <c r="W3" s="7"/>
@@ -1231,22 +1237,23 @@
       <c r="AE3" s="7"/>
       <c r="AF3" s="7"/>
       <c r="AG3" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="AH3" s="8"/>
+      <c r="AI3" s="7"/>
       <c r="AJ3" s="10"/>
       <c r="AK3" s="10"/>
+      <c r="AL3" s="10"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
@@ -1278,22 +1285,23 @@
       <c r="AE4" s="7"/>
       <c r="AF4" s="7"/>
       <c r="AG4" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="AH4" s="8"/>
+      <c r="AI4" s="7"/>
       <c r="AJ4" s="10"/>
       <c r="AK4" s="10"/>
+      <c r="AL4" s="10"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
@@ -1325,22 +1333,23 @@
       <c r="AE5" s="7"/>
       <c r="AF5" s="7"/>
       <c r="AG5" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH5" s="7"/>
-      <c r="AI5" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="AH5" s="8"/>
+      <c r="AI5" s="7"/>
       <c r="AJ5" s="10"/>
       <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
@@ -1372,12 +1381,13 @@
       <c r="AE6" s="7"/>
       <c r="AF6" s="7"/>
       <c r="AG6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH6" s="7"/>
-      <c r="AI6" s="10"/>
+        <v>36</v>
+      </c>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="7"/>
       <c r="AJ6" s="10"/>
       <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="4"/>
@@ -1385,16 +1395,17 @@
       <c r="C7" s="4"/>
       <c r="M7" s="11"/>
       <c r="AG7" s="4"/>
+      <c r="AH7" s="4"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1406,7 +1417,7 @@
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
       <c r="M8" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
@@ -1428,26 +1439,28 @@
       <c r="AE8" s="14"/>
       <c r="AF8" s="14"/>
       <c r="AG8" s="13"/>
-      <c r="AH8" s="14"/>
+      <c r="AH8" s="13"/>
       <c r="AI8" s="14"/>
       <c r="AJ8" s="14"/>
       <c r="AK8" s="14"/>
+      <c r="AL8" s="14"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="AG9" s="4"/>
-      <c r="AI9" s="16"/>
+      <c r="AH9" s="4"/>
       <c r="AJ9" s="16"/>
       <c r="AK9" s="16"/>
+      <c r="AL9" s="16"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
@@ -1457,7 +1470,7 @@
       <c r="I10" s="19"/>
       <c r="J10" s="19"/>
       <c r="K10" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L10" s="19"/>
       <c r="M10" s="19"/>
@@ -1470,7 +1483,7 @@
       <c r="T10" s="19"/>
       <c r="U10" s="19"/>
       <c r="V10" s="20" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="W10" s="19"/>
       <c r="X10" s="19"/>
@@ -1484,19 +1497,20 @@
       <c r="AF10" s="19"/>
       <c r="AG10" s="19"/>
       <c r="AH10" s="19"/>
-      <c r="AI10" s="22"/>
+      <c r="AI10" s="19"/>
       <c r="AJ10" s="22"/>
       <c r="AK10" s="22"/>
+      <c r="AL10" s="22"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
@@ -1505,14 +1519,14 @@
       <c r="H11" s="19"/>
       <c r="I11" s="19"/>
       <c r="J11" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K11" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L11" s="19"/>
       <c r="M11" s="23" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="N11" s="19"/>
       <c r="O11" s="19"/>
@@ -1523,7 +1537,7 @@
       <c r="T11" s="19"/>
       <c r="U11" s="19"/>
       <c r="V11" s="20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="W11" s="19"/>
       <c r="X11" s="19"/>
@@ -1537,19 +1551,20 @@
       <c r="AF11" s="19"/>
       <c r="AG11" s="19"/>
       <c r="AH11" s="19"/>
-      <c r="AI11" s="22"/>
+      <c r="AI11" s="19"/>
       <c r="AJ11" s="22"/>
       <c r="AK11" s="22"/>
+      <c r="AL11" s="22"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
@@ -1558,12 +1573,12 @@
       <c r="H12" s="19"/>
       <c r="I12" s="19"/>
       <c r="J12" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K12" s="19"/>
       <c r="L12" s="19"/>
       <c r="M12" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N12" s="19"/>
       <c r="O12" s="19"/>
@@ -1574,7 +1589,7 @@
       <c r="T12" s="19"/>
       <c r="U12" s="19"/>
       <c r="V12" s="18" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="W12" s="19"/>
       <c r="X12" s="19"/>
@@ -1587,22 +1602,23 @@
       <c r="AE12" s="21"/>
       <c r="AF12" s="19"/>
       <c r="AG12" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH12" s="19"/>
-      <c r="AI12" s="22"/>
+      <c r="AI12" s="19"/>
       <c r="AJ12" s="22"/>
       <c r="AK12" s="22"/>
+      <c r="AL12" s="22"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
@@ -1614,7 +1630,7 @@
       <c r="K13" s="19"/>
       <c r="L13" s="19"/>
       <c r="M13" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N13" s="19"/>
       <c r="O13" s="19"/>
@@ -1637,19 +1653,20 @@
       <c r="AF13" s="19"/>
       <c r="AG13" s="19"/>
       <c r="AH13" s="19"/>
-      <c r="AI13" s="22"/>
+      <c r="AI13" s="19"/>
       <c r="AJ13" s="22"/>
       <c r="AK13" s="22"/>
+      <c r="AL13" s="22"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
@@ -1661,7 +1678,7 @@
       <c r="K14" s="19"/>
       <c r="L14" s="19"/>
       <c r="M14" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N14" s="19"/>
       <c r="O14" s="19"/>
@@ -1684,19 +1701,20 @@
       <c r="AF14" s="19"/>
       <c r="AG14" s="19"/>
       <c r="AH14" s="19"/>
-      <c r="AI14" s="22"/>
+      <c r="AI14" s="19"/>
       <c r="AJ14" s="22"/>
       <c r="AK14" s="22"/>
+      <c r="AL14" s="22"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
@@ -1708,7 +1726,7 @@
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
       <c r="M15" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N15" s="19"/>
       <c r="O15" s="19"/>
@@ -1730,22 +1748,23 @@
       <c r="AE15" s="19"/>
       <c r="AF15" s="19"/>
       <c r="AG15" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="AH15" s="19"/>
-      <c r="AI15" s="22"/>
+        <v>36</v>
+      </c>
+      <c r="AH15" s="18"/>
+      <c r="AI15" s="19"/>
       <c r="AJ15" s="22"/>
       <c r="AK15" s="22"/>
+      <c r="AL15" s="22"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
@@ -1757,7 +1776,7 @@
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
       <c r="M16" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N16" s="19"/>
       <c r="O16" s="19"/>
@@ -1779,22 +1798,23 @@
       <c r="AE16" s="19"/>
       <c r="AF16" s="19"/>
       <c r="AG16" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH16" s="19"/>
-      <c r="AI16" s="22"/>
+      <c r="AI16" s="19"/>
       <c r="AJ16" s="22"/>
       <c r="AK16" s="22"/>
+      <c r="AL16" s="22"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B17" s="25" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
@@ -1806,7 +1826,7 @@
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
       <c r="M17" s="19" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N17" s="19"/>
       <c r="O17" s="19"/>
@@ -1829,19 +1849,20 @@
       <c r="AF17" s="19"/>
       <c r="AG17" s="19"/>
       <c r="AH17" s="19"/>
-      <c r="AI17" s="22"/>
+      <c r="AI17" s="19"/>
       <c r="AJ17" s="22"/>
       <c r="AK17" s="22"/>
+      <c r="AL17" s="22"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B18" s="25" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
@@ -1853,7 +1874,7 @@
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
       <c r="M18" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N18" s="19"/>
       <c r="O18" s="19"/>
@@ -1876,13 +1897,14 @@
       <c r="AF18" s="19"/>
       <c r="AG18" s="19"/>
       <c r="AH18" s="19"/>
-      <c r="AI18" s="22"/>
+      <c r="AI18" s="19"/>
       <c r="AJ18" s="22"/>
       <c r="AK18" s="22"/>
+      <c r="AL18" s="22"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="27" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>69</v>
@@ -1900,7 +1922,7 @@
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
       <c r="M19" s="18" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N19" s="19"/>
       <c r="O19" s="19"/>
@@ -1922,10 +1944,13 @@
       <c r="AE19" s="26"/>
       <c r="AF19" s="19"/>
       <c r="AG19" s="19"/>
-      <c r="AH19" s="19"/>
-      <c r="AI19" s="22"/>
+      <c r="AH19" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI19" s="19"/>
       <c r="AJ19" s="22"/>
       <c r="AK19" s="22"/>
+      <c r="AL19" s="22"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="4"/>
@@ -1938,10 +1963,10 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="12" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
@@ -1978,6 +2003,7 @@
       <c r="AI21" s="14"/>
       <c r="AJ21" s="14"/>
       <c r="AK21" s="14"/>
+      <c r="AL21" s="14"/>
     </row>
     <row r="22" ht="15.75" customHeight="1"/>
     <row r="24" ht="15.75" customHeight="1"/>
@@ -2693,7 +2719,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>1</v>
@@ -4525,22 +4551,22 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B1" s="28" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D1" s="28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E1" s="28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F1" s="39" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G1" s="28"/>
       <c r="H1" s="28"/>
@@ -4564,21 +4590,21 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="40" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C2" s="42">
         <f>NOW()</f>
-        <v>44323.05588</v>
+        <v>44326.05695</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E2" s="36"/>
       <c r="F2" s="43" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G2" s="36"/>
       <c r="H2" s="36"/>
@@ -5604,7 +5630,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="28" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B1" s="28" t="s">
         <v>1</v>
@@ -5647,13 +5673,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D2" s="37"/>
       <c r="E2" s="37"/>
@@ -5678,13 +5704,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="37" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" s="37"/>
       <c r="E3" s="37"/>
@@ -5734,13 +5760,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D5" s="37"/>
       <c r="E5" s="37"/>
@@ -5765,13 +5791,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B6" s="37" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="D6" s="37"/>
       <c r="E6" s="37"/>
@@ -5796,13 +5822,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B7" s="37" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C7" s="37" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D7" s="37"/>
       <c r="E7" s="37"/>
@@ -5827,13 +5853,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B8" s="37" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C8" s="37" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
@@ -5858,13 +5884,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D9" s="37"/>
       <c r="E9" s="37"/>
@@ -5914,13 +5940,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B11" s="37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C11" s="37" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="37"/>
@@ -5945,13 +5971,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B12" s="37" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="37"/>
@@ -5976,13 +6002,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B13" s="37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C13" s="37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
@@ -6007,13 +6033,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B14" s="37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="37"/>
@@ -6038,13 +6064,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B15" s="37" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="37" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D15" s="37"/>
       <c r="E15" s="37"/>
@@ -6069,13 +6095,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="37" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C16" s="37" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D16" s="37"/>
       <c r="E16" s="37"/>
@@ -6125,13 +6151,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B18" s="37" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C18" s="37" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D18" s="37"/>
       <c r="E18" s="37"/>
@@ -6156,13 +6182,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B19" s="37" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C19" s="37" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D19" s="37"/>
       <c r="E19" s="37"/>
@@ -6187,13 +6213,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B20" s="37" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C20" s="37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D20" s="37"/>
       <c r="E20" s="37"/>
@@ -6218,13 +6244,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B21" s="37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C21" s="37" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D21" s="37"/>
       <c r="E21" s="37"/>
@@ -6249,13 +6275,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="37" t="s">
+        <v>112</v>
+      </c>
+      <c r="B22" s="37" t="s">
+        <v>110</v>
+      </c>
+      <c r="C22" s="37" t="s">
         <v>111</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>109</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>110</v>
       </c>
       <c r="D22" s="37"/>
       <c r="E22" s="37"/>
@@ -6280,13 +6306,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="37" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B23" s="37" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C23" s="37" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D23" s="37"/>
       <c r="E23" s="37"/>
@@ -6336,13 +6362,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B25" s="37" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C25" s="37" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="D25" s="37"/>
       <c r="E25" s="37"/>
@@ -6367,13 +6393,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B26" s="37" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C26" s="37" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
@@ -6398,13 +6424,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B27" s="37" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C27" s="37" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D27" s="37"/>
       <c r="E27" s="37"/>
@@ -6429,13 +6455,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B28" s="37" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C28" s="37" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D28" s="37"/>
       <c r="E28" s="37"/>
@@ -6460,13 +6486,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="37" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B29" s="37" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C29" s="37" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D29" s="37"/>
       <c r="E29" s="37"/>
@@ -6516,13 +6542,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B31" s="37" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C31" s="37" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D31" s="37"/>
       <c r="E31" s="37"/>
@@ -6547,13 +6573,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="37" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C32" s="37" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D32" s="37"/>
       <c r="E32" s="37"/>
@@ -6603,121 +6629,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B34" s="4" t="str">
         <f t="shared" ref="B34:B42" si="1">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B35" s="4" t="str">
         <f t="shared" si="1"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B36" s="4" t="str">
         <f t="shared" si="1"/>
         <v>injectibles</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B37" s="4" t="str">
         <f t="shared" si="1"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B38" s="4" t="str">
         <f t="shared" si="1"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B39" s="4" t="str">
         <f t="shared" si="1"/>
         <v>iud</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B40" s="4" t="str">
         <f t="shared" si="1"/>
         <v>condoms</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B41" s="4" t="str">
         <f t="shared" si="1"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B42" s="4" t="str">
         <f t="shared" si="1"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="4" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -6728,26 +6754,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B45" s="4" t="str">
         <f t="shared" si="2"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B46" s="4" t="str">
         <f t="shared" si="2"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -6758,13 +6784,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="44" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B48" s="44" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C48" s="44" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D48" s="44"/>
       <c r="E48" s="44"/>
@@ -6789,13 +6815,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="44" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B49" s="44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C49" s="44" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D49" s="44"/>
       <c r="E49" s="44"/>
@@ -6821,226 +6847,226 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="4" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B58" s="44" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C58" s="44" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B59" s="44" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C59" s="44" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B60" s="44" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C60" s="44" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="44" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B61" s="44" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C61" s="44" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="36" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B63" s="36" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C63" s="44" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="36" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B64" s="36" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C64" s="44" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="36" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B65" s="36" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C65" s="44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="36" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B66" s="36" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C66" s="44" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="36" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B67" s="36" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C67" s="44" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="4" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="4" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>